<commit_message>
check null and undefined for Model value
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1174" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1064" uniqueCount="31">
   <si>
     <t>src</t>
   </si>
@@ -1612,11 +1612,11 @@
       <c r="C44" s="1">
         <v>44815</v>
       </c>
-      <c r="D44" t="s">
-        <v>10</v>
-      </c>
-      <c r="E44" t="s">
-        <v>10</v>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
       </c>
       <c r="F44" t="s">
         <v>10</v>
@@ -1624,8 +1624,8 @@
       <c r="G44" t="s">
         <v>10</v>
       </c>
-      <c r="H44" t="s">
-        <v>10</v>
+      <c r="H44">
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -3874,11 +3874,11 @@
       <c r="C131" s="1">
         <v>44807</v>
       </c>
-      <c r="D131" t="s">
-        <v>10</v>
-      </c>
-      <c r="E131" t="s">
-        <v>10</v>
+      <c r="D131">
+        <v>0</v>
+      </c>
+      <c r="E131">
+        <v>0</v>
       </c>
       <c r="F131" t="s">
         <v>10</v>
@@ -3886,8 +3886,8 @@
       <c r="G131" t="s">
         <v>10</v>
       </c>
-      <c r="H131" t="s">
-        <v>10</v>
+      <c r="H131">
+        <v>0</v>
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.25">
@@ -4689,8 +4689,8 @@
       <c r="F162" t="s">
         <v>10</v>
       </c>
-      <c r="G162" t="s">
-        <v>10</v>
+      <c r="G162">
+        <v>0</v>
       </c>
       <c r="H162" t="s">
         <v>10</v>
@@ -5382,17 +5382,17 @@
       <c r="C189" s="1">
         <v>44742.70833333333</v>
       </c>
-      <c r="D189" t="s">
-        <v>10</v>
-      </c>
-      <c r="E189" t="s">
-        <v>10</v>
+      <c r="D189">
+        <v>0</v>
+      </c>
+      <c r="E189">
+        <v>0</v>
       </c>
       <c r="F189" t="s">
         <v>10</v>
       </c>
-      <c r="G189" t="s">
-        <v>10</v>
+      <c r="G189">
+        <v>0</v>
       </c>
       <c r="H189" t="s">
         <v>10</v>
@@ -5408,17 +5408,17 @@
       <c r="C190" s="1">
         <v>44743.70833333333</v>
       </c>
-      <c r="D190" t="s">
-        <v>10</v>
-      </c>
-      <c r="E190" t="s">
-        <v>10</v>
+      <c r="D190">
+        <v>0</v>
+      </c>
+      <c r="E190">
+        <v>0</v>
       </c>
       <c r="F190" t="s">
         <v>10</v>
       </c>
-      <c r="G190" t="s">
-        <v>10</v>
+      <c r="G190">
+        <v>0</v>
       </c>
       <c r="H190" t="s">
         <v>10</v>
@@ -5434,17 +5434,17 @@
       <c r="C191" s="1">
         <v>44744.70833333333</v>
       </c>
-      <c r="D191" t="s">
-        <v>10</v>
-      </c>
-      <c r="E191" t="s">
-        <v>10</v>
+      <c r="D191">
+        <v>0</v>
+      </c>
+      <c r="E191">
+        <v>0</v>
       </c>
       <c r="F191" t="s">
         <v>10</v>
       </c>
-      <c r="G191" t="s">
-        <v>10</v>
+      <c r="G191">
+        <v>0</v>
       </c>
       <c r="H191" t="s">
         <v>10</v>
@@ -5460,17 +5460,17 @@
       <c r="C192" s="1">
         <v>44745.70833333333</v>
       </c>
-      <c r="D192" t="s">
-        <v>10</v>
-      </c>
-      <c r="E192" t="s">
-        <v>10</v>
+      <c r="D192">
+        <v>0</v>
+      </c>
+      <c r="E192">
+        <v>0</v>
       </c>
       <c r="F192" t="s">
         <v>10</v>
       </c>
-      <c r="G192" t="s">
-        <v>10</v>
+      <c r="G192">
+        <v>0</v>
       </c>
       <c r="H192" t="s">
         <v>10</v>
@@ -5486,17 +5486,17 @@
       <c r="C193" s="1">
         <v>44746.70833333333</v>
       </c>
-      <c r="D193" t="s">
-        <v>10</v>
-      </c>
-      <c r="E193" t="s">
-        <v>10</v>
+      <c r="D193">
+        <v>0</v>
+      </c>
+      <c r="E193">
+        <v>0</v>
       </c>
       <c r="F193" t="s">
         <v>10</v>
       </c>
-      <c r="G193" t="s">
-        <v>10</v>
+      <c r="G193">
+        <v>0</v>
       </c>
       <c r="H193" t="s">
         <v>10</v>
@@ -5521,8 +5521,8 @@
       <c r="F194" t="s">
         <v>10</v>
       </c>
-      <c r="G194" t="s">
-        <v>10</v>
+      <c r="G194">
+        <v>0</v>
       </c>
       <c r="H194" t="s">
         <v>10</v>
@@ -5573,8 +5573,8 @@
       <c r="F196" t="s">
         <v>10</v>
       </c>
-      <c r="G196" t="s">
-        <v>10</v>
+      <c r="G196">
+        <v>0</v>
       </c>
       <c r="H196" t="s">
         <v>10</v>
@@ -5593,14 +5593,14 @@
       <c r="D197">
         <v>5</v>
       </c>
-      <c r="E197" t="s">
-        <v>10</v>
+      <c r="E197">
+        <v>0</v>
       </c>
       <c r="F197" t="s">
         <v>10</v>
       </c>
-      <c r="G197" t="s">
-        <v>10</v>
+      <c r="G197">
+        <v>0</v>
       </c>
       <c r="H197" t="s">
         <v>10</v>
@@ -5616,17 +5616,17 @@
       <c r="C198" s="1">
         <v>44751.70833333333</v>
       </c>
-      <c r="D198" t="s">
-        <v>10</v>
-      </c>
-      <c r="E198" t="s">
-        <v>10</v>
+      <c r="D198">
+        <v>0</v>
+      </c>
+      <c r="E198">
+        <v>0</v>
       </c>
       <c r="F198" t="s">
         <v>10</v>
       </c>
-      <c r="G198" t="s">
-        <v>10</v>
+      <c r="G198">
+        <v>0</v>
       </c>
       <c r="H198" t="s">
         <v>10</v>
@@ -5645,14 +5645,14 @@
       <c r="D199">
         <v>3</v>
       </c>
-      <c r="E199" t="s">
-        <v>10</v>
+      <c r="E199">
+        <v>0</v>
       </c>
       <c r="F199" t="s">
         <v>10</v>
       </c>
-      <c r="G199" t="s">
-        <v>10</v>
+      <c r="G199">
+        <v>0</v>
       </c>
       <c r="H199" t="s">
         <v>10</v>
@@ -5677,8 +5677,8 @@
       <c r="F200" t="s">
         <v>10</v>
       </c>
-      <c r="G200" t="s">
-        <v>10</v>
+      <c r="G200">
+        <v>0</v>
       </c>
       <c r="H200" t="s">
         <v>10</v>
@@ -5703,8 +5703,8 @@
       <c r="F201" t="s">
         <v>10</v>
       </c>
-      <c r="G201" t="s">
-        <v>10</v>
+      <c r="G201">
+        <v>0</v>
       </c>
       <c r="H201" t="s">
         <v>10</v>
@@ -5723,14 +5723,14 @@
       <c r="D202">
         <v>29</v>
       </c>
-      <c r="E202" t="s">
-        <v>10</v>
+      <c r="E202">
+        <v>0</v>
       </c>
       <c r="F202" t="s">
         <v>10</v>
       </c>
-      <c r="G202" t="s">
-        <v>10</v>
+      <c r="G202">
+        <v>0</v>
       </c>
       <c r="H202" t="s">
         <v>10</v>
@@ -5749,14 +5749,14 @@
       <c r="D203">
         <v>20</v>
       </c>
-      <c r="E203" t="s">
-        <v>10</v>
+      <c r="E203">
+        <v>0</v>
       </c>
       <c r="F203" t="s">
         <v>10</v>
       </c>
-      <c r="G203" t="s">
-        <v>10</v>
+      <c r="G203">
+        <v>0</v>
       </c>
       <c r="H203" t="s">
         <v>10</v>
@@ -5775,14 +5775,14 @@
       <c r="D204">
         <v>40</v>
       </c>
-      <c r="E204" t="s">
-        <v>10</v>
+      <c r="E204">
+        <v>0</v>
       </c>
       <c r="F204" t="s">
         <v>10</v>
       </c>
-      <c r="G204" t="s">
-        <v>10</v>
+      <c r="G204">
+        <v>0</v>
       </c>
       <c r="H204" t="s">
         <v>10</v>
@@ -5801,14 +5801,14 @@
       <c r="D205">
         <v>6</v>
       </c>
-      <c r="E205" t="s">
-        <v>10</v>
+      <c r="E205">
+        <v>0</v>
       </c>
       <c r="F205" t="s">
         <v>10</v>
       </c>
-      <c r="G205" t="s">
-        <v>10</v>
+      <c r="G205">
+        <v>0</v>
       </c>
       <c r="H205" t="s">
         <v>10</v>
@@ -5827,14 +5827,14 @@
       <c r="D206">
         <v>13</v>
       </c>
-      <c r="E206" t="s">
-        <v>10</v>
+      <c r="E206">
+        <v>0</v>
       </c>
       <c r="F206" t="s">
         <v>10</v>
       </c>
-      <c r="G206" t="s">
-        <v>10</v>
+      <c r="G206">
+        <v>0</v>
       </c>
       <c r="H206" t="s">
         <v>10</v>
@@ -5853,14 +5853,14 @@
       <c r="D207">
         <v>20</v>
       </c>
-      <c r="E207" t="s">
-        <v>10</v>
+      <c r="E207">
+        <v>0</v>
       </c>
       <c r="F207" t="s">
         <v>10</v>
       </c>
-      <c r="G207" t="s">
-        <v>10</v>
+      <c r="G207">
+        <v>0</v>
       </c>
       <c r="H207" t="s">
         <v>10</v>
@@ -5879,14 +5879,14 @@
       <c r="D208">
         <v>12</v>
       </c>
-      <c r="E208" t="s">
-        <v>10</v>
+      <c r="E208">
+        <v>0</v>
       </c>
       <c r="F208" t="s">
         <v>10</v>
       </c>
-      <c r="G208" t="s">
-        <v>10</v>
+      <c r="G208">
+        <v>0</v>
       </c>
       <c r="H208" t="s">
         <v>10</v>
@@ -5911,8 +5911,8 @@
       <c r="F209" t="s">
         <v>10</v>
       </c>
-      <c r="G209" t="s">
-        <v>10</v>
+      <c r="G209">
+        <v>0</v>
       </c>
       <c r="H209" t="s">
         <v>10</v>
@@ -5931,14 +5931,14 @@
       <c r="D210">
         <v>11</v>
       </c>
-      <c r="E210" t="s">
-        <v>10</v>
+      <c r="E210">
+        <v>0</v>
       </c>
       <c r="F210" t="s">
         <v>10</v>
       </c>
-      <c r="G210" t="s">
-        <v>10</v>
+      <c r="G210">
+        <v>0</v>
       </c>
       <c r="H210" t="s">
         <v>10</v>
@@ -5957,14 +5957,14 @@
       <c r="D211">
         <v>3</v>
       </c>
-      <c r="E211" t="s">
-        <v>10</v>
+      <c r="E211">
+        <v>0</v>
       </c>
       <c r="F211" t="s">
         <v>10</v>
       </c>
-      <c r="G211" t="s">
-        <v>10</v>
+      <c r="G211">
+        <v>0</v>
       </c>
       <c r="H211" t="s">
         <v>10</v>
@@ -5983,14 +5983,14 @@
       <c r="D212">
         <v>2</v>
       </c>
-      <c r="E212" t="s">
-        <v>10</v>
+      <c r="E212">
+        <v>0</v>
       </c>
       <c r="F212" t="s">
         <v>10</v>
       </c>
-      <c r="G212" t="s">
-        <v>10</v>
+      <c r="G212">
+        <v>0</v>
       </c>
       <c r="H212" t="s">
         <v>10</v>
@@ -6015,8 +6015,8 @@
       <c r="F213" t="s">
         <v>10</v>
       </c>
-      <c r="G213" t="s">
-        <v>10</v>
+      <c r="G213">
+        <v>0</v>
       </c>
       <c r="H213" t="s">
         <v>10</v>
@@ -6041,8 +6041,8 @@
       <c r="F214" t="s">
         <v>10</v>
       </c>
-      <c r="G214" t="s">
-        <v>10</v>
+      <c r="G214">
+        <v>0</v>
       </c>
       <c r="H214" t="s">
         <v>10</v>
@@ -6067,8 +6067,8 @@
       <c r="F215" t="s">
         <v>10</v>
       </c>
-      <c r="G215" t="s">
-        <v>10</v>
+      <c r="G215">
+        <v>0</v>
       </c>
       <c r="H215" t="s">
         <v>10</v>
@@ -6087,14 +6087,14 @@
       <c r="D216">
         <v>9</v>
       </c>
-      <c r="E216" t="s">
-        <v>10</v>
+      <c r="E216">
+        <v>0</v>
       </c>
       <c r="F216" t="s">
         <v>10</v>
       </c>
-      <c r="G216" t="s">
-        <v>10</v>
+      <c r="G216">
+        <v>0</v>
       </c>
       <c r="H216" t="s">
         <v>10</v>
@@ -6113,14 +6113,14 @@
       <c r="D217">
         <v>9</v>
       </c>
-      <c r="E217" t="s">
-        <v>10</v>
+      <c r="E217">
+        <v>0</v>
       </c>
       <c r="F217" t="s">
         <v>10</v>
       </c>
-      <c r="G217" t="s">
-        <v>10</v>
+      <c r="G217">
+        <v>0</v>
       </c>
       <c r="H217" t="s">
         <v>10</v>
@@ -6145,8 +6145,8 @@
       <c r="F218" t="s">
         <v>10</v>
       </c>
-      <c r="G218" t="s">
-        <v>10</v>
+      <c r="G218">
+        <v>0</v>
       </c>
       <c r="H218" t="s">
         <v>10</v>
@@ -6165,14 +6165,14 @@
       <c r="D219">
         <v>25</v>
       </c>
-      <c r="E219" t="s">
-        <v>10</v>
+      <c r="E219">
+        <v>0</v>
       </c>
       <c r="F219" t="s">
         <v>10</v>
       </c>
-      <c r="G219" t="s">
-        <v>10</v>
+      <c r="G219">
+        <v>0</v>
       </c>
       <c r="H219" t="s">
         <v>10</v>
@@ -6191,14 +6191,14 @@
       <c r="D220">
         <v>8</v>
       </c>
-      <c r="E220" t="s">
-        <v>10</v>
+      <c r="E220">
+        <v>0</v>
       </c>
       <c r="F220" t="s">
         <v>10</v>
       </c>
-      <c r="G220" t="s">
-        <v>10</v>
+      <c r="G220">
+        <v>0</v>
       </c>
       <c r="H220" t="s">
         <v>10</v>
@@ -6223,8 +6223,8 @@
       <c r="F221" t="s">
         <v>10</v>
       </c>
-      <c r="G221" t="s">
-        <v>10</v>
+      <c r="G221">
+        <v>0</v>
       </c>
       <c r="H221" t="s">
         <v>10</v>
@@ -6243,14 +6243,14 @@
       <c r="D222">
         <v>57</v>
       </c>
-      <c r="E222" t="s">
-        <v>10</v>
+      <c r="E222">
+        <v>0</v>
       </c>
       <c r="F222" t="s">
         <v>10</v>
       </c>
-      <c r="G222" t="s">
-        <v>10</v>
+      <c r="G222">
+        <v>0</v>
       </c>
       <c r="H222" t="s">
         <v>10</v>
@@ -6269,14 +6269,14 @@
       <c r="D223">
         <v>34</v>
       </c>
-      <c r="E223" t="s">
-        <v>10</v>
+      <c r="E223">
+        <v>0</v>
       </c>
       <c r="F223" t="s">
         <v>10</v>
       </c>
-      <c r="G223" t="s">
-        <v>10</v>
+      <c r="G223">
+        <v>0</v>
       </c>
       <c r="H223" t="s">
         <v>10</v>
@@ -6301,8 +6301,8 @@
       <c r="F224" t="s">
         <v>10</v>
       </c>
-      <c r="G224" t="s">
-        <v>10</v>
+      <c r="G224">
+        <v>0</v>
       </c>
       <c r="H224" t="s">
         <v>10</v>
@@ -6327,8 +6327,8 @@
       <c r="F225" t="s">
         <v>10</v>
       </c>
-      <c r="G225" t="s">
-        <v>10</v>
+      <c r="G225">
+        <v>0</v>
       </c>
       <c r="H225" t="s">
         <v>10</v>
@@ -6347,14 +6347,14 @@
       <c r="D226">
         <v>27</v>
       </c>
-      <c r="E226" t="s">
-        <v>10</v>
+      <c r="E226">
+        <v>0</v>
       </c>
       <c r="F226" t="s">
         <v>10</v>
       </c>
-      <c r="G226" t="s">
-        <v>10</v>
+      <c r="G226">
+        <v>0</v>
       </c>
       <c r="H226" t="s">
         <v>10</v>
@@ -6431,8 +6431,8 @@
       <c r="F229" t="s">
         <v>10</v>
       </c>
-      <c r="G229" t="s">
-        <v>10</v>
+      <c r="G229">
+        <v>0</v>
       </c>
       <c r="H229" t="s">
         <v>10</v>
@@ -6483,8 +6483,8 @@
       <c r="F231" t="s">
         <v>10</v>
       </c>
-      <c r="G231" t="s">
-        <v>10</v>
+      <c r="G231">
+        <v>0</v>
       </c>
       <c r="H231" t="s">
         <v>10</v>
@@ -6535,8 +6535,8 @@
       <c r="F233" t="s">
         <v>10</v>
       </c>
-      <c r="G233" t="s">
-        <v>10</v>
+      <c r="G233">
+        <v>0</v>
       </c>
       <c r="H233" t="s">
         <v>10</v>
@@ -6581,14 +6581,14 @@
       <c r="D235">
         <v>33</v>
       </c>
-      <c r="E235" t="s">
-        <v>10</v>
+      <c r="E235">
+        <v>0</v>
       </c>
       <c r="F235" t="s">
         <v>10</v>
       </c>
-      <c r="G235" t="s">
-        <v>10</v>
+      <c r="G235">
+        <v>0</v>
       </c>
       <c r="H235" t="s">
         <v>10</v>
@@ -6607,14 +6607,14 @@
       <c r="D236">
         <v>52</v>
       </c>
-      <c r="E236" t="s">
-        <v>10</v>
+      <c r="E236">
+        <v>0</v>
       </c>
       <c r="F236" t="s">
         <v>10</v>
       </c>
-      <c r="G236" t="s">
-        <v>10</v>
+      <c r="G236">
+        <v>0</v>
       </c>
       <c r="H236" t="s">
         <v>10</v>
@@ -6639,8 +6639,8 @@
       <c r="F237" t="s">
         <v>10</v>
       </c>
-      <c r="G237" t="s">
-        <v>10</v>
+      <c r="G237">
+        <v>0</v>
       </c>
       <c r="H237" t="s">
         <v>10</v>
@@ -6665,8 +6665,8 @@
       <c r="F238" t="s">
         <v>10</v>
       </c>
-      <c r="G238" t="s">
-        <v>10</v>
+      <c r="G238">
+        <v>0</v>
       </c>
       <c r="H238" t="s">
         <v>10</v>
@@ -6685,14 +6685,14 @@
       <c r="D239">
         <v>128</v>
       </c>
-      <c r="E239" t="s">
-        <v>10</v>
+      <c r="E239">
+        <v>0</v>
       </c>
       <c r="F239" t="s">
         <v>10</v>
       </c>
-      <c r="G239" t="s">
-        <v>10</v>
+      <c r="G239">
+        <v>0</v>
       </c>
       <c r="H239" t="s">
         <v>10</v>
@@ -6717,8 +6717,8 @@
       <c r="F240" t="s">
         <v>10</v>
       </c>
-      <c r="G240" t="s">
-        <v>10</v>
+      <c r="G240">
+        <v>0</v>
       </c>
       <c r="H240" t="s">
         <v>10</v>
@@ -6763,14 +6763,14 @@
       <c r="D242">
         <v>24</v>
       </c>
-      <c r="E242" t="s">
-        <v>10</v>
+      <c r="E242">
+        <v>0</v>
       </c>
       <c r="F242" t="s">
         <v>10</v>
       </c>
-      <c r="G242" t="s">
-        <v>10</v>
+      <c r="G242">
+        <v>0</v>
       </c>
       <c r="H242" t="s">
         <v>10</v>
@@ -6815,14 +6815,14 @@
       <c r="D244">
         <v>23</v>
       </c>
-      <c r="E244" t="s">
-        <v>10</v>
+      <c r="E244">
+        <v>0</v>
       </c>
       <c r="F244" t="s">
         <v>10</v>
       </c>
-      <c r="G244" t="s">
-        <v>10</v>
+      <c r="G244">
+        <v>0</v>
       </c>
       <c r="H244" t="s">
         <v>10</v>
@@ -6847,8 +6847,8 @@
       <c r="F245" t="s">
         <v>10</v>
       </c>
-      <c r="G245" t="s">
-        <v>10</v>
+      <c r="G245">
+        <v>0</v>
       </c>
       <c r="H245" t="s">
         <v>10</v>
@@ -6873,8 +6873,8 @@
       <c r="F246" t="s">
         <v>10</v>
       </c>
-      <c r="G246" t="s">
-        <v>10</v>
+      <c r="G246">
+        <v>0</v>
       </c>
       <c r="H246" t="s">
         <v>10</v>
@@ -6899,8 +6899,8 @@
       <c r="F247" t="s">
         <v>10</v>
       </c>
-      <c r="G247" t="s">
-        <v>10</v>
+      <c r="G247">
+        <v>0</v>
       </c>
       <c r="H247" t="s">
         <v>10</v>
@@ -6925,8 +6925,8 @@
       <c r="F248" t="s">
         <v>10</v>
       </c>
-      <c r="G248" t="s">
-        <v>10</v>
+      <c r="G248">
+        <v>0</v>
       </c>
       <c r="H248" t="s">
         <v>10</v>
@@ -6951,8 +6951,8 @@
       <c r="F249" t="s">
         <v>10</v>
       </c>
-      <c r="G249" t="s">
-        <v>10</v>
+      <c r="G249">
+        <v>0</v>
       </c>
       <c r="H249" t="s">
         <v>10</v>
@@ -6977,8 +6977,8 @@
       <c r="F250" t="s">
         <v>10</v>
       </c>
-      <c r="G250" t="s">
-        <v>10</v>
+      <c r="G250">
+        <v>0</v>
       </c>
       <c r="H250" t="s">
         <v>10</v>
@@ -7003,8 +7003,8 @@
       <c r="F251" t="s">
         <v>10</v>
       </c>
-      <c r="G251" t="s">
-        <v>10</v>
+      <c r="G251">
+        <v>0</v>
       </c>
       <c r="H251" t="s">
         <v>10</v>
@@ -7029,8 +7029,8 @@
       <c r="F252" t="s">
         <v>10</v>
       </c>
-      <c r="G252" t="s">
-        <v>10</v>
+      <c r="G252">
+        <v>0</v>
       </c>
       <c r="H252" t="s">
         <v>10</v>
@@ -7055,8 +7055,8 @@
       <c r="F253" t="s">
         <v>10</v>
       </c>
-      <c r="G253" t="s">
-        <v>10</v>
+      <c r="G253">
+        <v>0</v>
       </c>
       <c r="H253" t="s">
         <v>10</v>
@@ -7081,8 +7081,8 @@
       <c r="F254" t="s">
         <v>10</v>
       </c>
-      <c r="G254" t="s">
-        <v>10</v>
+      <c r="G254">
+        <v>0</v>
       </c>
       <c r="H254" t="s">
         <v>10</v>
@@ -7107,8 +7107,8 @@
       <c r="F255" t="s">
         <v>10</v>
       </c>
-      <c r="G255" t="s">
-        <v>10</v>
+      <c r="G255">
+        <v>0</v>
       </c>
       <c r="H255" t="s">
         <v>10</v>
@@ -7133,8 +7133,8 @@
       <c r="F256" t="s">
         <v>10</v>
       </c>
-      <c r="G256" t="s">
-        <v>10</v>
+      <c r="G256">
+        <v>0</v>
       </c>
       <c r="H256" t="s">
         <v>10</v>
@@ -7159,8 +7159,8 @@
       <c r="F257" t="s">
         <v>10</v>
       </c>
-      <c r="G257" t="s">
-        <v>10</v>
+      <c r="G257">
+        <v>0</v>
       </c>
       <c r="H257" t="s">
         <v>10</v>
@@ -7185,8 +7185,8 @@
       <c r="F258" t="s">
         <v>10</v>
       </c>
-      <c r="G258" t="s">
-        <v>10</v>
+      <c r="G258">
+        <v>0</v>
       </c>
       <c r="H258" t="s">
         <v>10</v>
@@ -7237,8 +7237,8 @@
       <c r="F260" t="s">
         <v>10</v>
       </c>
-      <c r="G260" t="s">
-        <v>10</v>
+      <c r="G260">
+        <v>0</v>
       </c>
       <c r="H260" t="s">
         <v>10</v>
@@ -7263,8 +7263,8 @@
       <c r="F261" t="s">
         <v>10</v>
       </c>
-      <c r="G261" t="s">
-        <v>10</v>
+      <c r="G261">
+        <v>0</v>
       </c>
       <c r="H261" t="s">
         <v>10</v>
@@ -7289,8 +7289,8 @@
       <c r="F262" t="s">
         <v>10</v>
       </c>
-      <c r="G262" t="s">
-        <v>10</v>
+      <c r="G262">
+        <v>0</v>
       </c>
       <c r="H262" t="s">
         <v>10</v>
@@ -7341,8 +7341,8 @@
       <c r="F264" t="s">
         <v>10</v>
       </c>
-      <c r="G264" t="s">
-        <v>10</v>
+      <c r="G264">
+        <v>0</v>
       </c>
       <c r="H264" t="s">
         <v>10</v>
@@ -7367,8 +7367,8 @@
       <c r="F265" t="s">
         <v>10</v>
       </c>
-      <c r="G265" t="s">
-        <v>10</v>
+      <c r="G265">
+        <v>0</v>
       </c>
       <c r="H265" t="s">
         <v>10</v>

</xml_diff>